<commit_message>
Added Cingulata cleaned by François
</commit_message>
<xml_diff>
--- a/data_2023/cleaning_Xenarthra/Cingulata_FP_2.0.xlsx
+++ b/data_2023/cleaning_Xenarthra/Cingulata_FP_2.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Internship_ISEM\Neotropical_Mammals\REPO\Neotropical_mammals\data_2023\cleaning_Xenarthra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AFB1250-460B-44AB-843A-7C2F3CB82C7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50BEF832-9B77-4D61-A69F-CA1413D0AE2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{1F93D83E-7E3D-4018-B28A-94D1C7F51376}"/>
   </bookViews>
@@ -3535,9 +3535,6 @@
     <t>Stegotherium_variegatum</t>
   </si>
   <si>
-    <t>tegotherium</t>
-  </si>
-  <si>
     <t>Los Cardones</t>
   </si>
   <si>
@@ -5811,6 +5808,9 @@
       </rPr>
       <t xml:space="preserve"> cf. tuberculatus</t>
     </r>
+  </si>
+  <si>
+    <t>Noatherium</t>
   </si>
 </sst>
 </file>
@@ -6306,7 +6306,7 @@
   <dimension ref="A1:O1467"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6372,7 +6372,7 @@
         <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>1161</v>
+        <v>1438</v>
       </c>
       <c r="D2" t="s">
         <v>17</v>
@@ -6387,13 +6387,13 @@
         <v>20</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>1161</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>1162</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" t="s">
         <v>1163</v>
-      </c>
-      <c r="J2" t="s">
-        <v>1164</v>
       </c>
       <c r="K2" s="1">
         <v>46.2</v>
@@ -6440,7 +6440,7 @@
         <v>29</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="K3" s="1">
         <v>39</v>
@@ -6481,10 +6481,10 @@
         <v>20</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="J4" t="s">
         <v>34</v>
@@ -6516,7 +6516,7 @@
         <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>18</v>
@@ -6531,10 +6531,10 @@
         <v>1144</v>
       </c>
       <c r="I5" s="1" t="s">
+        <v>1167</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>1168</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>1169</v>
       </c>
       <c r="K5" s="1">
         <v>30</v>
@@ -6575,13 +6575,13 @@
         <v>162</v>
       </c>
       <c r="H6" s="1" t="s">
+        <v>1169</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>1170</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>1171</v>
-      </c>
       <c r="J6" s="1" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="K6" s="1">
         <v>30</v>
@@ -6704,7 +6704,7 @@
         <v>51</v>
       </c>
       <c r="D9" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="E9" t="s">
         <v>16</v>
@@ -6716,7 +6716,7 @@
         <v>57</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="I9" t="s">
         <v>16</v>
@@ -6798,7 +6798,7 @@
         <v>51</v>
       </c>
       <c r="D11" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="E11" t="s">
         <v>16</v>
@@ -6831,7 +6831,7 @@
         <v>55</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
@@ -6857,7 +6857,7 @@
         <v>72</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>58</v>
@@ -6875,7 +6875,7 @@
         <v>66</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
@@ -6907,7 +6907,7 @@
         <v>16</v>
       </c>
       <c r="J13" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="K13" s="1">
         <v>1.1999999999999999E-3</v>
@@ -7403,7 +7403,7 @@
         <v>51</v>
       </c>
       <c r="D24" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="E24" t="s">
         <v>69</v>
@@ -7562,7 +7562,7 @@
         <v>16</v>
       </c>
       <c r="J27" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="K27" s="1">
         <v>1.17E-2</v>
@@ -7732,7 +7732,7 @@
         <v>51</v>
       </c>
       <c r="D31" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="E31" t="s">
         <v>69</v>
@@ -7750,7 +7750,7 @@
         <v>113</v>
       </c>
       <c r="J31" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="K31" s="1">
         <v>0.3</v>
@@ -7797,7 +7797,7 @@
         <v>118</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
       <c r="K32" s="1">
         <v>9.07</v>
@@ -7812,7 +7812,7 @@
         <v>22</v>
       </c>
       <c r="O32" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.3">
@@ -8023,7 +8023,7 @@
         <v>72</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="I37" t="s">
         <v>16</v>
@@ -8044,7 +8044,7 @@
         <v>66</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.3">
@@ -9339,7 +9339,7 @@
         <v>165</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="I65" s="1" t="s">
         <v>244</v>
@@ -10737,7 +10737,7 @@
         <v>205</v>
       </c>
       <c r="D95" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="E95" t="s">
         <v>16</v>
@@ -10937,7 +10937,7 @@
         <v>153</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="I99" t="s">
         <v>16</v>
@@ -10990,7 +10990,7 @@
         <v>16</v>
       </c>
       <c r="J100" s="1" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="K100" s="1">
         <v>16.5</v>
@@ -11031,7 +11031,7 @@
         <v>162</v>
       </c>
       <c r="H101" s="1" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="I101" s="1" t="s">
         <v>162</v>
@@ -11078,7 +11078,7 @@
         <v>162</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="I102" s="1" t="s">
         <v>162</v>
@@ -11125,7 +11125,7 @@
         <v>162</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="I103" s="1" t="s">
         <v>162</v>
@@ -11219,13 +11219,13 @@
         <v>165</v>
       </c>
       <c r="H105" s="1" t="s">
+        <v>1190</v>
+      </c>
+      <c r="I105" t="s">
+        <v>16</v>
+      </c>
+      <c r="J105" s="1" t="s">
         <v>1191</v>
-      </c>
-      <c r="I105" t="s">
-        <v>16</v>
-      </c>
-      <c r="J105" s="1" t="s">
-        <v>1192</v>
       </c>
       <c r="K105" s="1">
         <v>23.03</v>
@@ -11254,7 +11254,7 @@
         <v>205</v>
       </c>
       <c r="D106" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="E106" t="s">
         <v>16</v>
@@ -11301,7 +11301,7 @@
         <v>205</v>
       </c>
       <c r="D107" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="E107" t="s">
         <v>16</v>
@@ -11407,7 +11407,7 @@
         <v>162</v>
       </c>
       <c r="H109" s="1" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="I109" s="1" t="s">
         <v>162</v>
@@ -11442,7 +11442,7 @@
         <v>205</v>
       </c>
       <c r="D110" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="E110" t="s">
         <v>16</v>
@@ -11501,10 +11501,10 @@
         <v>165</v>
       </c>
       <c r="H111" s="1" t="s">
+        <v>1194</v>
+      </c>
+      <c r="I111" s="1" t="s">
         <v>1195</v>
-      </c>
-      <c r="I111" s="1" t="s">
-        <v>1196</v>
       </c>
       <c r="J111" s="1" t="s">
         <v>160</v>
@@ -11595,7 +11595,7 @@
         <v>220</v>
       </c>
       <c r="H113" s="1" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="I113" t="s">
         <v>16</v>
@@ -11616,7 +11616,7 @@
         <v>55</v>
       </c>
       <c r="O113" s="1" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.3">
@@ -11642,7 +11642,7 @@
         <v>177</v>
       </c>
       <c r="H114" s="1" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="I114" t="s">
         <v>16</v>
@@ -11689,7 +11689,7 @@
         <v>177</v>
       </c>
       <c r="H115" s="1" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="I115" t="s">
         <v>16</v>
@@ -12679,7 +12679,7 @@
         <v>248</v>
       </c>
       <c r="I136" s="1" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="J136" s="1" t="s">
         <v>163</v>
@@ -12773,7 +12773,7 @@
         <v>154</v>
       </c>
       <c r="I138" s="1" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="J138" t="s">
         <v>155</v>
@@ -12820,7 +12820,7 @@
         <v>213</v>
       </c>
       <c r="I139" s="1" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="J139" t="s">
         <v>163</v>
@@ -12852,7 +12852,7 @@
         <v>230</v>
       </c>
       <c r="D140" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="E140" t="s">
         <v>16</v>
@@ -12958,7 +12958,7 @@
         <v>157</v>
       </c>
       <c r="H142" s="1" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="I142" t="s">
         <v>16</v>
@@ -13005,10 +13005,10 @@
         <v>153</v>
       </c>
       <c r="H143" s="1" t="s">
+        <v>1205</v>
+      </c>
+      <c r="I143" s="1" t="s">
         <v>1206</v>
-      </c>
-      <c r="I143" s="1" t="s">
-        <v>1207</v>
       </c>
       <c r="J143" t="s">
         <v>160</v>
@@ -13052,7 +13052,7 @@
         <v>162</v>
       </c>
       <c r="H144" s="1" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="I144" s="1" t="s">
         <v>162</v>
@@ -13099,7 +13099,7 @@
         <v>162</v>
       </c>
       <c r="H145" s="1" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="I145" s="1" t="s">
         <v>162</v>
@@ -13146,7 +13146,7 @@
         <v>162</v>
       </c>
       <c r="H146" s="1" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="I146" s="1" t="s">
         <v>162</v>
@@ -13319,7 +13319,7 @@
         <v>230</v>
       </c>
       <c r="D150" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="E150" t="s">
         <v>16</v>
@@ -13331,7 +13331,7 @@
         <v>165</v>
       </c>
       <c r="H150" s="1" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="I150" t="s">
         <v>16</v>
@@ -13472,10 +13472,10 @@
         <v>100</v>
       </c>
       <c r="H153" s="1" t="s">
+        <v>1209</v>
+      </c>
+      <c r="I153" s="1" t="s">
         <v>1210</v>
-      </c>
-      <c r="I153" s="1" t="s">
-        <v>1211</v>
       </c>
       <c r="J153" t="s">
         <v>54</v>
@@ -13519,7 +13519,7 @@
         <v>162</v>
       </c>
       <c r="H154" s="1" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="I154" s="1" t="s">
         <v>162</v>
@@ -13613,7 +13613,7 @@
         <v>165</v>
       </c>
       <c r="H156" s="1" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="I156" t="s">
         <v>16</v>
@@ -13666,7 +13666,7 @@
         <v>16</v>
       </c>
       <c r="J157" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="K157" s="1">
         <v>5.3330000000000002</v>
@@ -13713,7 +13713,7 @@
         <v>16</v>
       </c>
       <c r="J158" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="K158" s="1">
         <v>11.5</v>
@@ -13751,13 +13751,13 @@
         <v>176</v>
       </c>
       <c r="G159" s="1" t="s">
+        <v>1214</v>
+      </c>
+      <c r="H159" s="1" t="s">
         <v>1215</v>
       </c>
-      <c r="H159" s="1" t="s">
-        <v>1216</v>
-      </c>
       <c r="I159" s="1" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="J159" t="s">
         <v>163</v>
@@ -13804,7 +13804,7 @@
         <v>188</v>
       </c>
       <c r="J160" s="1" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="K160" s="1">
         <v>20</v>
@@ -14133,7 +14133,7 @@
         <v>191</v>
       </c>
       <c r="J167" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="K167" s="1">
         <v>20</v>
@@ -14503,7 +14503,7 @@
         <v>162</v>
       </c>
       <c r="H175" s="1" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="I175" s="1" t="s">
         <v>162</v>
@@ -14600,7 +14600,7 @@
         <v>16</v>
       </c>
       <c r="J177" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="K177" s="1">
         <v>15.5</v>
@@ -14647,7 +14647,7 @@
         <v>16</v>
       </c>
       <c r="J178" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="K178" s="1">
         <v>0</v>
@@ -14694,7 +14694,7 @@
         <v>16</v>
       </c>
       <c r="J179" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="K179" s="1">
         <v>0.3</v>
@@ -14788,7 +14788,7 @@
         <v>16</v>
       </c>
       <c r="J181" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="K181">
         <v>1.17E-2</v>
@@ -14829,7 +14829,7 @@
         <v>76</v>
       </c>
       <c r="H182" s="1" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="I182" t="s">
         <v>16</v>
@@ -14882,7 +14882,7 @@
         <v>16</v>
       </c>
       <c r="J183" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="K183">
         <v>0</v>
@@ -14923,7 +14923,7 @@
         <v>76</v>
       </c>
       <c r="H184" s="1" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="I184" t="s">
         <v>16</v>
@@ -14970,13 +14970,13 @@
         <v>255</v>
       </c>
       <c r="H185" s="1" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="I185" t="s">
         <v>16</v>
       </c>
       <c r="J185" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="K185" s="1">
         <v>1.17E-2</v>
@@ -15017,13 +15017,13 @@
         <v>87</v>
       </c>
       <c r="H186" s="1" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="I186" t="s">
         <v>16</v>
       </c>
       <c r="J186" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="K186">
         <v>1.17E-2</v>
@@ -15064,7 +15064,7 @@
         <v>76</v>
       </c>
       <c r="H187" s="1" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="I187" t="s">
         <v>16</v>
@@ -15111,13 +15111,13 @@
         <v>121</v>
       </c>
       <c r="H188" s="1" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="I188" t="s">
         <v>16</v>
       </c>
       <c r="J188" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="K188" s="1">
         <v>1.17E-2</v>
@@ -15164,7 +15164,7 @@
         <v>16</v>
       </c>
       <c r="J189" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="K189">
         <v>1.17E-2</v>
@@ -15193,7 +15193,7 @@
         <v>250</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="E190" t="s">
         <v>16</v>
@@ -15240,7 +15240,7 @@
         <v>250</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="E191" t="s">
         <v>16</v>
@@ -15252,7 +15252,7 @@
         <v>76</v>
       </c>
       <c r="H191" s="1" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="I191" t="s">
         <v>16</v>
@@ -15287,7 +15287,7 @@
         <v>250</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="E192" t="s">
         <v>16</v>
@@ -15334,7 +15334,7 @@
         <v>250</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="E193" t="s">
         <v>16</v>
@@ -15346,7 +15346,7 @@
         <v>255</v>
       </c>
       <c r="H193" s="1" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="I193" t="s">
         <v>16</v>
@@ -15381,7 +15381,7 @@
         <v>250</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="E194" t="s">
         <v>16</v>
@@ -15393,13 +15393,13 @@
         <v>16</v>
       </c>
       <c r="H194" s="1" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="I194" t="s">
         <v>16</v>
       </c>
       <c r="J194" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="K194" s="1">
         <v>1.17E-2</v>
@@ -15414,7 +15414,7 @@
         <v>66</v>
       </c>
       <c r="O194" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="195" spans="1:15" x14ac:dyDescent="0.3">
@@ -15487,13 +15487,13 @@
         <v>266</v>
       </c>
       <c r="H196" s="1" t="s">
+        <v>1233</v>
+      </c>
+      <c r="I196" t="s">
+        <v>16</v>
+      </c>
+      <c r="J196" t="s">
         <v>1234</v>
-      </c>
-      <c r="I196" t="s">
-        <v>16</v>
-      </c>
-      <c r="J196" t="s">
-        <v>1235</v>
       </c>
       <c r="K196" s="1">
         <v>5.3330000000000002</v>
@@ -15540,7 +15540,7 @@
         <v>273</v>
       </c>
       <c r="J197" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="K197" s="1">
         <v>5.3330000000000002</v>
@@ -15581,7 +15581,7 @@
         <v>278</v>
       </c>
       <c r="H198" s="1" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="I198" t="s">
         <v>16</v>
@@ -15628,7 +15628,7 @@
         <v>278</v>
       </c>
       <c r="H199" s="4" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="I199" s="2" t="s">
         <v>16</v>
@@ -15675,7 +15675,7 @@
         <v>278</v>
       </c>
       <c r="H200" s="4" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="I200" s="2" t="s">
         <v>16</v>
@@ -15722,7 +15722,7 @@
         <v>278</v>
       </c>
       <c r="H201" s="4" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="I201" s="2" t="s">
         <v>16</v>
@@ -15769,7 +15769,7 @@
         <v>278</v>
       </c>
       <c r="H202" s="4" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="I202" s="2" t="s">
         <v>16</v>
@@ -15816,7 +15816,7 @@
         <v>165</v>
       </c>
       <c r="H203" s="1" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="I203" t="s">
         <v>16</v>
@@ -15869,7 +15869,7 @@
         <v>16</v>
       </c>
       <c r="J204" s="6" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="K204" s="6">
         <v>23.03</v>
@@ -16004,7 +16004,7 @@
         <v>165</v>
       </c>
       <c r="H207" s="1" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="I207" t="s">
         <v>16</v>
@@ -16054,10 +16054,10 @@
         <v>285</v>
       </c>
       <c r="I208" s="1" t="s">
+        <v>1239</v>
+      </c>
+      <c r="J208" t="s">
         <v>1240</v>
-      </c>
-      <c r="J208" t="s">
-        <v>1241</v>
       </c>
       <c r="K208" s="1">
         <v>30</v>
@@ -16086,7 +16086,7 @@
         <v>284</v>
       </c>
       <c r="D209" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="E209" t="s">
         <v>16</v>
@@ -16098,13 +16098,13 @@
         <v>165</v>
       </c>
       <c r="H209" s="1" t="s">
+        <v>1242</v>
+      </c>
+      <c r="I209" t="s">
+        <v>16</v>
+      </c>
+      <c r="J209" t="s">
         <v>1243</v>
-      </c>
-      <c r="I209" t="s">
-        <v>16</v>
-      </c>
-      <c r="J209" t="s">
-        <v>1244</v>
       </c>
       <c r="K209" s="1">
         <v>47.8</v>
@@ -16148,10 +16148,10 @@
         <v>16</v>
       </c>
       <c r="I210" s="1" t="s">
+        <v>1239</v>
+      </c>
+      <c r="J210" t="s">
         <v>1240</v>
-      </c>
-      <c r="J210" t="s">
-        <v>1241</v>
       </c>
       <c r="K210" s="1">
         <v>30</v>
@@ -16245,7 +16245,7 @@
         <v>211</v>
       </c>
       <c r="J212" s="2" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="K212" s="4">
         <v>30</v>
@@ -16386,7 +16386,7 @@
         <v>16</v>
       </c>
       <c r="J215" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="K215" s="1">
         <v>30</v>
@@ -16574,7 +16574,7 @@
         <v>16</v>
       </c>
       <c r="J219" s="2" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="K219" s="4">
         <v>28.4</v>
@@ -16621,7 +16621,7 @@
         <v>16</v>
       </c>
       <c r="J220" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="K220" s="1">
         <v>30</v>
@@ -16665,7 +16665,7 @@
         <v>303</v>
       </c>
       <c r="I221" s="1" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="J221" t="s">
         <v>54</v>
@@ -16712,7 +16712,7 @@
         <v>303</v>
       </c>
       <c r="I222" s="4" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="J222" s="4" t="s">
         <v>54</v>
@@ -16759,7 +16759,7 @@
         <v>306</v>
       </c>
       <c r="I223" s="1" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="J223" t="s">
         <v>54</v>
@@ -16947,7 +16947,7 @@
         <v>312</v>
       </c>
       <c r="I227" s="1" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="J227" t="s">
         <v>54</v>
@@ -16965,7 +16965,7 @@
         <v>22</v>
       </c>
       <c r="O227" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="228" spans="1:15" x14ac:dyDescent="0.3">
@@ -17088,7 +17088,7 @@
         <v>303</v>
       </c>
       <c r="I230" s="1" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="J230" t="s">
         <v>54</v>
@@ -17135,7 +17135,7 @@
         <v>303</v>
       </c>
       <c r="I231" s="4" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="J231" s="2" t="s">
         <v>54</v>
@@ -17323,7 +17323,7 @@
         <v>322</v>
       </c>
       <c r="I235" s="1" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="J235" t="s">
         <v>119</v>
@@ -17370,7 +17370,7 @@
         <v>323</v>
       </c>
       <c r="I236" s="1" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="J236" t="s">
         <v>119</v>
@@ -18474,7 +18474,7 @@
         <v>346</v>
       </c>
       <c r="H260" s="1" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="I260" s="1" t="s">
         <v>1143</v>
@@ -18556,7 +18556,7 @@
         <v>348</v>
       </c>
       <c r="D262" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="E262" t="s">
         <v>16</v>
@@ -18574,7 +18574,7 @@
         <v>16</v>
       </c>
       <c r="J262" s="1" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="K262" s="8">
         <v>3.3</v>
@@ -18709,10 +18709,10 @@
         <v>60</v>
       </c>
       <c r="H265" s="1" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="I265" s="1" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="J265" t="s">
         <v>54</v>
@@ -18759,7 +18759,7 @@
         <v>16</v>
       </c>
       <c r="I266" s="1" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="J266" t="s">
         <v>355</v>
@@ -19044,7 +19044,7 @@
         <v>362</v>
       </c>
       <c r="J272" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="K272" s="1">
         <v>3.6</v>
@@ -19085,7 +19085,7 @@
         <v>70</v>
       </c>
       <c r="H273" s="1" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="I273" t="s">
         <v>16</v>
@@ -19185,7 +19185,7 @@
         <v>16</v>
       </c>
       <c r="J275" s="2" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="K275" s="4">
         <v>3.6</v>
@@ -19414,7 +19414,7 @@
         <v>16</v>
       </c>
       <c r="J280" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="K280" s="1">
         <v>3.6</v>
@@ -20040,7 +20040,7 @@
         <v>49</v>
       </c>
       <c r="O293" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="294" spans="1:15" x14ac:dyDescent="0.3">
@@ -20536,10 +20536,10 @@
         <v>100</v>
       </c>
       <c r="H304" s="1" t="s">
+        <v>1209</v>
+      </c>
+      <c r="I304" s="1" t="s">
         <v>1210</v>
-      </c>
-      <c r="I304" s="1" t="s">
-        <v>1211</v>
       </c>
       <c r="J304" t="s">
         <v>54</v>
@@ -20636,7 +20636,7 @@
         <v>16</v>
       </c>
       <c r="J306" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="K306" s="1">
         <v>1.17E-2</v>
@@ -20865,7 +20865,7 @@
         <v>136</v>
       </c>
       <c r="H311" s="1" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="I311" t="s">
         <v>16</v>
@@ -20959,13 +20959,13 @@
         <v>390</v>
       </c>
       <c r="H313" s="1" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="I313" t="s">
         <v>16</v>
       </c>
       <c r="J313" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="K313" s="1">
         <v>1.17E-2</v>
@@ -21053,7 +21053,7 @@
         <v>76</v>
       </c>
       <c r="H315" s="1" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="I315" t="s">
         <v>16</v>
@@ -21135,7 +21135,7 @@
         <v>394</v>
       </c>
       <c r="D317" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="E317" t="s">
         <v>16</v>
@@ -21144,7 +21144,7 @@
         <v>61</v>
       </c>
       <c r="H317" s="1" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="I317" t="s">
         <v>16</v>
@@ -21273,7 +21273,7 @@
         <v>394</v>
       </c>
       <c r="D320" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="E320" t="s">
         <v>16</v>
@@ -21332,7 +21332,7 @@
         <v>131</v>
       </c>
       <c r="H321" s="1" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="I321" t="s">
         <v>16</v>
@@ -21379,7 +21379,7 @@
         <v>121</v>
       </c>
       <c r="H322" s="1" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="I322" t="s">
         <v>16</v>
@@ -21614,13 +21614,13 @@
         <v>150</v>
       </c>
       <c r="H327" s="1" t="s">
+        <v>1267</v>
+      </c>
+      <c r="I327" t="s">
+        <v>16</v>
+      </c>
+      <c r="J327" s="1" t="s">
         <v>1268</v>
-      </c>
-      <c r="I327" t="s">
-        <v>16</v>
-      </c>
-      <c r="J327" s="1" t="s">
-        <v>1269</v>
       </c>
       <c r="K327">
         <v>0</v>
@@ -21755,7 +21755,7 @@
         <v>403</v>
       </c>
       <c r="H330" s="1" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="I330" t="s">
         <v>16</v>
@@ -22025,7 +22025,7 @@
         <v>411</v>
       </c>
       <c r="D336" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="E336" t="s">
         <v>16</v>
@@ -22272,7 +22272,7 @@
         <v>215</v>
       </c>
       <c r="H341" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="I341" t="s">
         <v>16</v>
@@ -22307,7 +22307,7 @@
         <v>411</v>
       </c>
       <c r="D342" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="E342" t="s">
         <v>16</v>
@@ -22542,7 +22542,7 @@
         <v>411</v>
       </c>
       <c r="D347" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="E347" t="s">
         <v>18</v>
@@ -22889,7 +22889,7 @@
         <v>16</v>
       </c>
       <c r="J354" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="K354" s="1">
         <v>2.5880000000000001</v>
@@ -23638,7 +23638,7 @@
         <v>373</v>
       </c>
       <c r="J370" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="K370" s="1">
         <v>4</v>
@@ -23779,7 +23779,7 @@
         <v>438</v>
       </c>
       <c r="J373" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="K373" s="1">
         <v>4</v>
@@ -24008,7 +24008,7 @@
         <v>76</v>
       </c>
       <c r="H378" s="1" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="I378" s="1" t="s">
         <v>360</v>
@@ -24432,10 +24432,10 @@
         <v>16</v>
       </c>
       <c r="I387" s="1" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="J387" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="K387">
         <v>1.17E-2</v>
@@ -24511,7 +24511,7 @@
         <v>443</v>
       </c>
       <c r="D389" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="E389" t="s">
         <v>18</v>
@@ -24558,7 +24558,7 @@
         <v>443</v>
       </c>
       <c r="D390" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="E390" t="s">
         <v>18</v>
@@ -24605,7 +24605,7 @@
         <v>443</v>
       </c>
       <c r="D391" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="E391" t="s">
         <v>18</v>
@@ -24652,7 +24652,7 @@
         <v>443</v>
       </c>
       <c r="D392" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="E392" t="s">
         <v>18</v>
@@ -24699,7 +24699,7 @@
         <v>443</v>
       </c>
       <c r="D393" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="E393" t="s">
         <v>18</v>
@@ -24746,7 +24746,7 @@
         <v>443</v>
       </c>
       <c r="D394" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="E394" t="s">
         <v>18</v>
@@ -24793,7 +24793,7 @@
         <v>443</v>
       </c>
       <c r="D395" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="E395" t="s">
         <v>18</v>
@@ -24993,7 +24993,7 @@
         <v>76</v>
       </c>
       <c r="H399" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="I399" t="s">
         <v>16</v>
@@ -25375,7 +25375,7 @@
         <v>16</v>
       </c>
       <c r="J407" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="K407" s="1">
         <v>0.3</v>
@@ -25416,10 +25416,10 @@
         <v>255</v>
       </c>
       <c r="H408" s="1" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="I408" s="1" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="J408" t="s">
         <v>79</v>
@@ -25557,7 +25557,7 @@
         <v>76</v>
       </c>
       <c r="H411" s="1" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="I411" t="s">
         <v>16</v>
@@ -25704,7 +25704,7 @@
         <v>472</v>
       </c>
       <c r="J414" s="1" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="K414" s="1">
         <v>48</v>
@@ -25792,7 +25792,7 @@
         <v>165</v>
       </c>
       <c r="H416" s="1" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="I416" t="s">
         <v>16</v>
@@ -25939,7 +25939,7 @@
         <v>29</v>
       </c>
       <c r="J419" s="1" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="K419" s="1">
         <v>39</v>
@@ -26156,7 +26156,7 @@
         <v>474</v>
       </c>
       <c r="D424" s="1" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="E424" t="s">
         <v>18</v>
@@ -26189,7 +26189,7 @@
         <v>114</v>
       </c>
       <c r="O424" s="1" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="425" spans="1:15" x14ac:dyDescent="0.3">
@@ -26221,7 +26221,7 @@
         <v>16</v>
       </c>
       <c r="J425" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="K425" s="1">
         <v>37.200000000000003</v>
@@ -26597,7 +26597,7 @@
         <v>16</v>
       </c>
       <c r="J433" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="K433" s="1">
         <v>5.3330000000000002</v>
@@ -26738,7 +26738,7 @@
         <v>16</v>
       </c>
       <c r="J436" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="K436">
         <v>5.3330000000000002</v>
@@ -26832,7 +26832,7 @@
         <v>16</v>
       </c>
       <c r="J438" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="K438" s="1">
         <v>3.3</v>
@@ -26879,7 +26879,7 @@
         <v>421</v>
       </c>
       <c r="J439" s="1" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="K439">
         <v>3.3</v>
@@ -27020,7 +27020,7 @@
         <v>16</v>
       </c>
       <c r="J442" s="2" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="K442" s="2">
         <v>6.8</v>
@@ -27114,7 +27114,7 @@
         <v>495</v>
       </c>
       <c r="J444" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="K444" s="1">
         <v>5.3330000000000002</v>
@@ -27161,7 +27161,7 @@
         <v>16</v>
       </c>
       <c r="J445" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="K445" s="1">
         <v>4</v>
@@ -27208,7 +27208,7 @@
         <v>315</v>
       </c>
       <c r="J446" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="K446" s="1">
         <v>9</v>
@@ -27490,7 +27490,7 @@
         <v>369</v>
       </c>
       <c r="J452" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="K452" s="1">
         <v>4</v>
@@ -28101,7 +28101,7 @@
         <v>16</v>
       </c>
       <c r="J465" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="K465">
         <v>3.3</v>
@@ -28148,7 +28148,7 @@
         <v>16</v>
       </c>
       <c r="J466" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="K466">
         <v>3.3</v>
@@ -29229,7 +29229,7 @@
         <v>510</v>
       </c>
       <c r="J489" s="2" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="K489" s="4">
         <v>36</v>
@@ -29276,7 +29276,7 @@
         <v>211</v>
       </c>
       <c r="J490" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="K490" s="1">
         <v>36</v>
@@ -29352,7 +29352,7 @@
         <v>512</v>
       </c>
       <c r="D492" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="E492" t="s">
         <v>16</v>
@@ -29399,7 +29399,7 @@
         <v>512</v>
       </c>
       <c r="D493" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="E493" t="s">
         <v>16</v>
@@ -29411,7 +29411,7 @@
         <v>165</v>
       </c>
       <c r="H493" s="1" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="I493" t="s">
         <v>16</v>
@@ -29446,7 +29446,7 @@
         <v>512</v>
       </c>
       <c r="D494" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="E494" t="s">
         <v>16</v>
@@ -29458,7 +29458,7 @@
         <v>165</v>
       </c>
       <c r="H494" s="1" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="I494" t="s">
         <v>16</v>
@@ -29493,7 +29493,7 @@
         <v>512</v>
       </c>
       <c r="D495" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="E495" t="s">
         <v>16</v>
@@ -29505,7 +29505,7 @@
         <v>165</v>
       </c>
       <c r="H495" s="1" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="I495" t="s">
         <v>16</v>
@@ -29540,7 +29540,7 @@
         <v>512</v>
       </c>
       <c r="D496" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="E496" t="s">
         <v>16</v>
@@ -29552,7 +29552,7 @@
         <v>162</v>
       </c>
       <c r="H496" s="1" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="I496" t="s">
         <v>16</v>
@@ -29587,7 +29587,7 @@
         <v>512</v>
       </c>
       <c r="D497" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="E497" t="s">
         <v>16</v>
@@ -29634,7 +29634,7 @@
         <v>512</v>
       </c>
       <c r="D498" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="E498" t="s">
         <v>16</v>
@@ -29681,7 +29681,7 @@
         <v>512</v>
       </c>
       <c r="D499" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="E499" t="s">
         <v>16</v>
@@ -29728,7 +29728,7 @@
         <v>512</v>
       </c>
       <c r="D500" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="E500" t="s">
         <v>16</v>
@@ -29790,7 +29790,7 @@
         <v>29</v>
       </c>
       <c r="J501" s="1" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="K501" s="1">
         <v>39</v>
@@ -29819,7 +29819,7 @@
         <v>512</v>
       </c>
       <c r="D502" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="E502" t="s">
         <v>18</v>
@@ -29866,7 +29866,7 @@
         <v>512</v>
       </c>
       <c r="D503" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="E503" t="s">
         <v>18</v>
@@ -29907,7 +29907,7 @@
         <v>512</v>
       </c>
       <c r="D504" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="E504" t="s">
         <v>18</v>
@@ -29919,7 +29919,7 @@
         <v>165</v>
       </c>
       <c r="H504" s="1" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="J504" s="1" t="s">
         <v>207</v>
@@ -29951,7 +29951,7 @@
         <v>512</v>
       </c>
       <c r="D505" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="E505" t="s">
         <v>18</v>
@@ -29998,7 +29998,7 @@
         <v>512</v>
       </c>
       <c r="D506" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="E506" t="s">
         <v>18</v>
@@ -30010,7 +30010,7 @@
         <v>165</v>
       </c>
       <c r="H506" s="1" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="I506" t="s">
         <v>16</v>
@@ -30045,7 +30045,7 @@
         <v>512</v>
       </c>
       <c r="D507" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="E507" t="s">
         <v>18</v>
@@ -30057,7 +30057,7 @@
         <v>298</v>
       </c>
       <c r="H507" s="1" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="I507" s="1"/>
       <c r="J507" s="1" t="s">
@@ -30090,7 +30090,7 @@
         <v>512</v>
       </c>
       <c r="D508" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="E508" t="s">
         <v>18</v>
@@ -30102,7 +30102,7 @@
         <v>165</v>
       </c>
       <c r="H508" s="1" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="I508" t="s">
         <v>16</v>
@@ -30137,16 +30137,16 @@
         <v>512</v>
       </c>
       <c r="D509" t="s">
+        <v>1304</v>
+      </c>
+      <c r="E509" t="s">
+        <v>18</v>
+      </c>
+      <c r="F509" s="1" t="s">
         <v>1305</v>
       </c>
-      <c r="E509" t="s">
-        <v>18</v>
-      </c>
-      <c r="F509" s="1" t="s">
+      <c r="H509" t="s">
         <v>1306</v>
-      </c>
-      <c r="H509" t="s">
-        <v>1307</v>
       </c>
       <c r="J509" s="1" t="s">
         <v>234</v>
@@ -30337,7 +30337,7 @@
         <v>16</v>
       </c>
       <c r="J513" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="K513" s="1">
         <v>36</v>
@@ -30425,7 +30425,7 @@
         <v>16</v>
       </c>
       <c r="H515" s="1" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="I515" t="s">
         <v>16</v>
@@ -30566,7 +30566,7 @@
         <v>70</v>
       </c>
       <c r="H518" s="1" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="I518" t="s">
         <v>16</v>
@@ -30895,10 +30895,10 @@
         <v>60</v>
       </c>
       <c r="H525" s="1" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="I525" s="1" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="J525" t="s">
         <v>54</v>
@@ -31465,7 +31465,7 @@
         <v>16</v>
       </c>
       <c r="J537" s="1" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="K537" s="1">
         <v>28.1</v>
@@ -31600,13 +31600,13 @@
         <v>16</v>
       </c>
       <c r="H540" s="1" t="s">
+        <v>1310</v>
+      </c>
+      <c r="I540" t="s">
+        <v>16</v>
+      </c>
+      <c r="J540" t="s">
         <v>1311</v>
-      </c>
-      <c r="I540" t="s">
-        <v>16</v>
-      </c>
-      <c r="J540" t="s">
-        <v>1312</v>
       </c>
       <c r="K540" s="1">
         <v>30</v>
@@ -31700,7 +31700,7 @@
         <v>29</v>
       </c>
       <c r="J542" s="1" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="K542" s="1">
         <v>39</v>
@@ -31747,7 +31747,7 @@
         <v>510</v>
       </c>
       <c r="J543" s="2" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="K543" s="4">
         <v>36</v>
@@ -31794,7 +31794,7 @@
         <v>211</v>
       </c>
       <c r="J544" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="K544" s="1">
         <v>36</v>
@@ -31841,7 +31841,7 @@
         <v>16</v>
       </c>
       <c r="J545" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="K545" s="1">
         <v>36</v>
@@ -31935,7 +31935,7 @@
         <v>211</v>
       </c>
       <c r="J547" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="K547" s="1">
         <v>30</v>
@@ -32023,7 +32023,7 @@
         <v>165</v>
       </c>
       <c r="H549" s="1" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="I549" t="s">
         <v>16</v>
@@ -32067,7 +32067,7 @@
         <v>176</v>
       </c>
       <c r="H550" s="1" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="I550" t="s">
         <v>16</v>
@@ -32120,7 +32120,7 @@
         <v>16</v>
       </c>
       <c r="J551" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="K551" s="1">
         <v>36</v>
@@ -32261,7 +32261,7 @@
         <v>16</v>
       </c>
       <c r="J554" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="K554" s="1">
         <v>41.2</v>
@@ -32308,7 +32308,7 @@
         <v>16</v>
       </c>
       <c r="J555" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="K555" s="1">
         <v>36</v>
@@ -32355,7 +32355,7 @@
         <v>16</v>
       </c>
       <c r="J556" s="2" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="K556" s="4">
         <v>11.5</v>
@@ -32684,7 +32684,7 @@
         <v>16</v>
       </c>
       <c r="J563" s="1" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="K563" s="1">
         <v>3.3</v>
@@ -32713,7 +32713,7 @@
         <v>557</v>
       </c>
       <c r="D564" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="E564" t="s">
         <v>16</v>
@@ -32854,7 +32854,7 @@
         <v>557</v>
       </c>
       <c r="D567" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="E567" t="s">
         <v>16</v>
@@ -33765,7 +33765,7 @@
         <v>16</v>
       </c>
       <c r="J586" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="K586" s="1">
         <v>11.5</v>
@@ -33859,7 +33859,7 @@
         <v>16</v>
       </c>
       <c r="J588" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="K588" s="1">
         <v>0.3</v>
@@ -33900,13 +33900,13 @@
         <v>87</v>
       </c>
       <c r="H589" s="1" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="I589" t="s">
         <v>16</v>
       </c>
       <c r="J589" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="K589" s="1">
         <v>1.17E-2</v>
@@ -34088,7 +34088,7 @@
         <v>16</v>
       </c>
       <c r="H593" s="1" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="I593" t="s">
         <v>16</v>
@@ -34229,7 +34229,7 @@
         <v>16</v>
       </c>
       <c r="H596" s="1" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="I596" t="s">
         <v>16</v>
@@ -34273,7 +34273,7 @@
         <v>110</v>
       </c>
       <c r="H597" s="1" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="I597" t="s">
         <v>16</v>
@@ -34320,7 +34320,7 @@
         <v>16</v>
       </c>
       <c r="H598" s="1" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="I598" t="s">
         <v>16</v>
@@ -35454,7 +35454,7 @@
         <v>16</v>
       </c>
       <c r="J622" s="1" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
       <c r="K622" s="1">
         <v>1.8</v>
@@ -35548,7 +35548,7 @@
         <v>16</v>
       </c>
       <c r="J624" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="K624" s="1">
         <v>36</v>
@@ -35642,7 +35642,7 @@
         <v>16</v>
       </c>
       <c r="J626" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="K626" s="1">
         <v>39</v>
@@ -35736,7 +35736,7 @@
         <v>16</v>
       </c>
       <c r="J628" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="K628" s="1">
         <v>39</v>
@@ -35783,7 +35783,7 @@
         <v>16</v>
       </c>
       <c r="J629" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="K629" s="1">
         <v>36</v>
@@ -35830,7 +35830,7 @@
         <v>16</v>
       </c>
       <c r="J630" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="K630" s="1">
         <v>39</v>
@@ -35859,7 +35859,7 @@
         <v>595</v>
       </c>
       <c r="D631" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="E631" t="s">
         <v>18</v>
@@ -35877,7 +35877,7 @@
         <v>603</v>
       </c>
       <c r="J631" s="1" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="K631" s="1">
         <v>44</v>
@@ -35924,7 +35924,7 @@
         <v>605</v>
       </c>
       <c r="J632" s="1" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="K632" s="1">
         <v>44</v>
@@ -35971,7 +35971,7 @@
         <v>16</v>
       </c>
       <c r="J633" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="K633" s="1">
         <v>39</v>
@@ -36065,7 +36065,7 @@
         <v>16</v>
       </c>
       <c r="J635" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="K635" s="1">
         <v>39</v>
@@ -36394,7 +36394,7 @@
         <v>16</v>
       </c>
       <c r="J642" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
       <c r="K642" s="1">
         <v>36</v>
@@ -36441,7 +36441,7 @@
         <v>16</v>
       </c>
       <c r="J643" s="2" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
       <c r="K643" s="2">
         <v>36.5</v>
@@ -36488,7 +36488,7 @@
         <v>16</v>
       </c>
       <c r="J644" s="2" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
       <c r="K644" s="2">
         <v>36.5</v>
@@ -36535,7 +36535,7 @@
         <v>16</v>
       </c>
       <c r="J645" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="K645" s="1">
         <v>39</v>
@@ -36582,7 +36582,7 @@
         <v>617</v>
       </c>
       <c r="J646" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
       <c r="K646" s="1">
         <v>36</v>
@@ -36723,7 +36723,7 @@
         <v>16</v>
       </c>
       <c r="J649" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="K649" s="1">
         <v>39</v>
@@ -36817,7 +36817,7 @@
         <v>16</v>
       </c>
       <c r="J651" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="K651" s="1">
         <v>44</v>
@@ -36864,7 +36864,7 @@
         <v>16</v>
       </c>
       <c r="J652" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="K652" s="1">
         <v>44</v>
@@ -36958,7 +36958,7 @@
         <v>16</v>
       </c>
       <c r="J654" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="K654" s="1">
         <v>39</v>
@@ -37099,7 +37099,7 @@
         <v>16</v>
       </c>
       <c r="J657" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
       <c r="K657" s="1">
         <v>51</v>
@@ -37475,7 +37475,7 @@
         <v>430</v>
       </c>
       <c r="J665" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="K665" s="1">
         <v>4</v>
@@ -37522,7 +37522,7 @@
         <v>16</v>
       </c>
       <c r="J666" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="K666" s="1">
         <v>1.8</v>
@@ -37569,7 +37569,7 @@
         <v>16</v>
       </c>
       <c r="J667" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="K667" s="1">
         <v>50</v>
@@ -37616,7 +37616,7 @@
         <v>16</v>
       </c>
       <c r="J668" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="K668" s="1">
         <v>47</v>
@@ -37898,7 +37898,7 @@
         <v>211</v>
       </c>
       <c r="J674" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="K674" s="1">
         <v>30</v>
@@ -37992,7 +37992,7 @@
         <v>16</v>
       </c>
       <c r="J676" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="K676" s="1">
         <v>47</v>
@@ -38039,7 +38039,7 @@
         <v>16</v>
       </c>
       <c r="J677" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="K677" s="1">
         <v>39</v>
@@ -38133,7 +38133,7 @@
         <v>16</v>
       </c>
       <c r="J679" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
       <c r="K679" s="9">
         <v>36</v>
@@ -38180,7 +38180,7 @@
         <v>16</v>
       </c>
       <c r="J680" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="K680" s="1">
         <v>36</v>
@@ -38227,7 +38227,7 @@
         <v>16</v>
       </c>
       <c r="J681" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="K681" s="1">
         <v>39</v>
@@ -38274,7 +38274,7 @@
         <v>16</v>
       </c>
       <c r="J682" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="K682" s="1">
         <v>39</v>
@@ -38368,7 +38368,7 @@
         <v>16</v>
       </c>
       <c r="J684" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="K684" s="1">
         <v>39</v>
@@ -38412,10 +38412,10 @@
         <v>16</v>
       </c>
       <c r="I685" s="1" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="J685" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="K685" s="1">
         <v>39</v>
@@ -38603,7 +38603,7 @@
         <v>16</v>
       </c>
       <c r="J689" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="K689" s="1">
         <v>39</v>
@@ -38650,7 +38650,7 @@
         <v>16</v>
       </c>
       <c r="J690" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="K690" s="1">
         <v>39</v>
@@ -38697,7 +38697,7 @@
         <v>16</v>
       </c>
       <c r="J691" s="2" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="K691" s="4">
         <v>39</v>
@@ -38744,7 +38744,7 @@
         <v>16</v>
       </c>
       <c r="J692" s="2" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="K692" s="4">
         <v>39</v>
@@ -38791,7 +38791,7 @@
         <v>16</v>
       </c>
       <c r="J693" s="2" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="K693" s="4">
         <v>39</v>
@@ -38838,7 +38838,7 @@
         <v>16</v>
       </c>
       <c r="J694" s="2" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="K694" s="4">
         <v>39</v>
@@ -38885,7 +38885,7 @@
         <v>16</v>
       </c>
       <c r="J695" s="2" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="K695" s="4">
         <v>39</v>
@@ -38932,7 +38932,7 @@
         <v>16</v>
       </c>
       <c r="J696" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="K696" s="1">
         <v>47</v>
@@ -38979,7 +38979,7 @@
         <v>16</v>
       </c>
       <c r="J697" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="K697" s="1">
         <v>39</v>
@@ -39026,7 +39026,7 @@
         <v>16</v>
       </c>
       <c r="J698" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="K698" s="1">
         <v>39</v>
@@ -39073,7 +39073,7 @@
         <v>16</v>
       </c>
       <c r="J699" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="K699" s="1">
         <v>39</v>
@@ -39167,7 +39167,7 @@
         <v>510</v>
       </c>
       <c r="J701" s="2" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="K701" s="4">
         <v>39</v>
@@ -39214,7 +39214,7 @@
         <v>211</v>
       </c>
       <c r="J702" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="K702" s="1">
         <v>39</v>
@@ -39261,7 +39261,7 @@
         <v>16</v>
       </c>
       <c r="J703" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="K703" s="1">
         <v>39</v>
@@ -39355,7 +39355,7 @@
         <v>16</v>
       </c>
       <c r="J705" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="K705" s="1">
         <v>39</v>
@@ -40060,7 +40060,7 @@
         <v>16</v>
       </c>
       <c r="J720" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="K720" s="1">
         <v>1.17E-2</v>
@@ -40154,7 +40154,7 @@
         <v>16</v>
       </c>
       <c r="J722" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="K722" s="1">
         <v>3.3</v>
@@ -40530,7 +40530,7 @@
         <v>16</v>
       </c>
       <c r="J730" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="K730" s="1">
         <v>0</v>
@@ -40718,7 +40718,7 @@
         <v>16</v>
       </c>
       <c r="J734" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="K734" s="1">
         <v>0</v>
@@ -40765,7 +40765,7 @@
         <v>16</v>
       </c>
       <c r="J735" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="K735" s="1">
         <v>0</v>
@@ -41229,7 +41229,7 @@
         <v>672</v>
       </c>
       <c r="H745" s="1" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="I745" t="s">
         <v>16</v>
@@ -41376,7 +41376,7 @@
         <v>16</v>
       </c>
       <c r="J748" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
       <c r="K748" s="1">
         <v>1.8</v>
@@ -42363,7 +42363,7 @@
         <v>693</v>
       </c>
       <c r="J769" s="1" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="K769" s="1">
         <v>3.3</v>
@@ -42407,10 +42407,10 @@
         <v>16</v>
       </c>
       <c r="I770" s="1" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="J770" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="K770" s="1">
         <v>11.5</v>
@@ -42639,7 +42639,7 @@
         <v>162</v>
       </c>
       <c r="H775" s="1" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="I775" s="1" t="s">
         <v>162</v>
@@ -43300,7 +43300,7 @@
         <v>712</v>
       </c>
       <c r="I789" s="1" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
       <c r="J789" t="s">
         <v>54</v>
@@ -43397,7 +43397,7 @@
         <v>16</v>
       </c>
       <c r="J791" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="K791" s="1">
         <v>0.3</v>
@@ -43538,7 +43538,7 @@
         <v>858</v>
       </c>
       <c r="J794" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="K794" s="1">
         <v>1.17E-2</v>
@@ -43585,7 +43585,7 @@
         <v>16</v>
       </c>
       <c r="J795" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
       <c r="K795" s="1">
         <v>0</v>
@@ -43679,7 +43679,7 @@
         <v>16</v>
       </c>
       <c r="J797" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="K797">
         <v>1.17E-2</v>
@@ -43773,7 +43773,7 @@
         <v>16</v>
       </c>
       <c r="J799" s="1" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="K799" s="1">
         <v>1.17E-2</v>
@@ -43820,7 +43820,7 @@
         <v>16</v>
       </c>
       <c r="J800" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="K800">
         <v>1.17E-2</v>
@@ -44149,7 +44149,7 @@
         <v>16</v>
       </c>
       <c r="J807" s="1" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="K807" s="1">
         <v>0</v>
@@ -44243,7 +44243,7 @@
         <v>16</v>
       </c>
       <c r="J809" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="K809">
         <v>4</v>
@@ -44410,10 +44410,10 @@
         <v>663</v>
       </c>
       <c r="C813" t="s">
+        <v>1349</v>
+      </c>
+      <c r="D813" t="s">
         <v>1350</v>
-      </c>
-      <c r="D813" t="s">
-        <v>1351</v>
       </c>
       <c r="E813" t="s">
         <v>18</v>
@@ -44431,7 +44431,7 @@
         <v>357</v>
       </c>
       <c r="J813" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="K813" s="1">
         <v>3.3</v>
@@ -44942,7 +44942,7 @@
         <v>47</v>
       </c>
       <c r="H824" s="1" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="I824" t="s">
         <v>16</v>
@@ -44974,10 +44974,10 @@
         <v>663</v>
       </c>
       <c r="C825" t="s">
+        <v>1353</v>
+      </c>
+      <c r="D825" t="s">
         <v>1354</v>
-      </c>
-      <c r="D825" t="s">
-        <v>1355</v>
       </c>
       <c r="E825" t="s">
         <v>18</v>
@@ -44995,7 +44995,7 @@
         <v>617</v>
       </c>
       <c r="J825" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="K825" s="1">
         <v>36</v>
@@ -45089,7 +45089,7 @@
         <v>16</v>
       </c>
       <c r="J827" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="K827" s="1">
         <v>4</v>
@@ -45165,7 +45165,7 @@
         <v>744</v>
       </c>
       <c r="D829" s="1" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="E829" t="s">
         <v>16</v>
@@ -45259,7 +45259,7 @@
         <v>744</v>
       </c>
       <c r="D831" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
       <c r="E831" t="s">
         <v>18</v>
@@ -45277,7 +45277,7 @@
         <v>357</v>
       </c>
       <c r="J831" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
       <c r="K831" s="1">
         <v>1.8</v>
@@ -46164,7 +46164,7 @@
         <v>162</v>
       </c>
       <c r="H850" s="1" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
       <c r="I850" t="s">
         <v>16</v>
@@ -46211,7 +46211,7 @@
         <v>162</v>
       </c>
       <c r="H851" s="1" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
       <c r="I851" t="s">
         <v>16</v>
@@ -46352,7 +46352,7 @@
         <v>762</v>
       </c>
       <c r="H854" s="1" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
       <c r="I854" t="s">
         <v>16</v>
@@ -46446,7 +46446,7 @@
         <v>501</v>
       </c>
       <c r="H856" s="1" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
       <c r="I856" t="s">
         <v>16</v>
@@ -46540,7 +46540,7 @@
         <v>76</v>
       </c>
       <c r="H858" s="1" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
       <c r="I858" t="s">
         <v>16</v>
@@ -46634,13 +46634,13 @@
         <v>76</v>
       </c>
       <c r="H860" s="1" t="s">
+        <v>1364</v>
+      </c>
+      <c r="I860" t="s">
+        <v>16</v>
+      </c>
+      <c r="J860" t="s">
         <v>1365</v>
-      </c>
-      <c r="I860" t="s">
-        <v>16</v>
-      </c>
-      <c r="J860" t="s">
-        <v>1366</v>
       </c>
       <c r="K860" s="1">
         <v>3.3</v>
@@ -46875,7 +46875,7 @@
         <v>16</v>
       </c>
       <c r="J865" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
       <c r="K865" s="1">
         <v>0</v>
@@ -47010,13 +47010,13 @@
         <v>215</v>
       </c>
       <c r="H868" s="1" t="s">
+        <v>1367</v>
+      </c>
+      <c r="I868" s="1" t="s">
         <v>1368</v>
       </c>
-      <c r="I868" s="1" t="s">
+      <c r="J868" s="1" t="s">
         <v>1369</v>
-      </c>
-      <c r="J868" s="1" t="s">
-        <v>1370</v>
       </c>
       <c r="K868">
         <v>1.2E-2</v>
@@ -47339,7 +47339,7 @@
         <v>124</v>
       </c>
       <c r="H875" s="1" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="I875" t="s">
         <v>16</v>
@@ -47374,7 +47374,7 @@
         <v>766</v>
       </c>
       <c r="D876" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
       <c r="E876" t="s">
         <v>16</v>
@@ -47386,7 +47386,7 @@
         <v>124</v>
       </c>
       <c r="H876" s="1" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
       <c r="I876" t="s">
         <v>16</v>
@@ -47433,7 +47433,7 @@
         <v>124</v>
       </c>
       <c r="H877" s="1" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
       <c r="I877" t="s">
         <v>16</v>
@@ -47468,7 +47468,7 @@
         <v>766</v>
       </c>
       <c r="D878" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="E878" t="s">
         <v>16</v>
@@ -47480,7 +47480,7 @@
         <v>124</v>
       </c>
       <c r="H878" s="1" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="I878" t="s">
         <v>16</v>
@@ -47610,10 +47610,10 @@
         <v>20</v>
       </c>
       <c r="H881" s="1" t="s">
+        <v>1375</v>
+      </c>
+      <c r="I881" s="1" t="s">
         <v>1376</v>
-      </c>
-      <c r="I881" s="1" t="s">
-        <v>1377</v>
       </c>
       <c r="J881" s="1" t="s">
         <v>79</v>
@@ -47645,7 +47645,7 @@
         <v>766</v>
       </c>
       <c r="D882" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
       <c r="E882" t="s">
         <v>16</v>
@@ -47692,7 +47692,7 @@
         <v>766</v>
       </c>
       <c r="D883" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="E883" t="s">
         <v>16</v>
@@ -47739,7 +47739,7 @@
         <v>766</v>
       </c>
       <c r="D884" s="1" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="E884" s="1"/>
       <c r="F884" s="1" t="s">
@@ -47833,7 +47833,7 @@
         <v>220</v>
       </c>
       <c r="H886" s="1" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="I886" t="s">
         <v>16</v>
@@ -47980,7 +47980,7 @@
         <v>16</v>
       </c>
       <c r="J889" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="K889" s="1">
         <v>0.3</v>
@@ -48074,7 +48074,7 @@
         <v>16</v>
       </c>
       <c r="J891" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="K891">
         <v>1.17E-2</v>
@@ -48356,7 +48356,7 @@
         <v>16</v>
       </c>
       <c r="J897" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="K897" s="1">
         <v>0</v>
@@ -48444,13 +48444,13 @@
         <v>780</v>
       </c>
       <c r="H899" s="1" t="s">
+        <v>1384</v>
+      </c>
+      <c r="I899" t="s">
+        <v>16</v>
+      </c>
+      <c r="J899" t="s">
         <v>1385</v>
-      </c>
-      <c r="I899" t="s">
-        <v>16</v>
-      </c>
-      <c r="J899" t="s">
-        <v>1386</v>
       </c>
       <c r="K899" s="1">
         <v>0</v>
@@ -48491,13 +48491,13 @@
         <v>782</v>
       </c>
       <c r="H900" s="1" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
       <c r="I900" t="s">
         <v>16</v>
       </c>
       <c r="J900" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="K900" s="1">
         <v>0</v>
@@ -48826,7 +48826,7 @@
         <v>16</v>
       </c>
       <c r="J907" s="2" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
       <c r="K907" s="4">
         <v>0</v>
@@ -48873,7 +48873,7 @@
         <v>16</v>
       </c>
       <c r="J908" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
       <c r="K908" s="1">
         <v>0</v>
@@ -48920,7 +48920,7 @@
         <v>16</v>
       </c>
       <c r="J909" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
       <c r="K909" s="1">
         <v>1.8</v>
@@ -49813,7 +49813,7 @@
         <v>16</v>
       </c>
       <c r="J928" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="K928" s="1">
         <v>0</v>
@@ -50559,7 +50559,7 @@
         <v>16</v>
       </c>
       <c r="H944" s="1" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
       <c r="I944" t="s">
         <v>16</v>
@@ -50653,7 +50653,7 @@
         <v>16</v>
       </c>
       <c r="H946" s="1" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="I946" t="s">
         <v>16</v>
@@ -50700,7 +50700,7 @@
         <v>16</v>
       </c>
       <c r="H947" s="1" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="I947" t="s">
         <v>16</v>
@@ -50747,7 +50747,7 @@
         <v>16</v>
       </c>
       <c r="H948" s="1" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="I948" t="s">
         <v>16</v>
@@ -51264,7 +51264,7 @@
         <v>76</v>
       </c>
       <c r="H959" s="1" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
       <c r="I959" t="s">
         <v>16</v>
@@ -51405,7 +51405,7 @@
         <v>76</v>
       </c>
       <c r="H962" s="1" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
       <c r="I962" t="s">
         <v>16</v>
@@ -51499,7 +51499,7 @@
         <v>76</v>
       </c>
       <c r="H964" s="1" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="I964" t="s">
         <v>16</v>
@@ -51546,7 +51546,7 @@
         <v>60</v>
       </c>
       <c r="H965" s="1" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
       <c r="I965" t="s">
         <v>16</v>
@@ -51593,7 +51593,7 @@
         <v>60</v>
       </c>
       <c r="H966" s="1" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="I966" t="s">
         <v>16</v>
@@ -51687,7 +51687,7 @@
         <v>416</v>
       </c>
       <c r="H968" s="1" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="I968" t="s">
         <v>16</v>
@@ -51734,7 +51734,7 @@
         <v>416</v>
       </c>
       <c r="H969" s="1" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
       <c r="I969" t="s">
         <v>16</v>
@@ -51781,7 +51781,7 @@
         <v>416</v>
       </c>
       <c r="H970" s="1" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
       <c r="I970" t="s">
         <v>16</v>
@@ -51828,7 +51828,7 @@
         <v>416</v>
       </c>
       <c r="H971" s="1" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="I971" t="s">
         <v>16</v>
@@ -51875,7 +51875,7 @@
         <v>475</v>
       </c>
       <c r="H972" s="1" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="I972" t="s">
         <v>16</v>
@@ -52063,7 +52063,7 @@
         <v>831</v>
       </c>
       <c r="H976" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
       <c r="I976" t="s">
         <v>16</v>
@@ -52110,7 +52110,7 @@
         <v>831</v>
       </c>
       <c r="H977" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
       <c r="I977" t="s">
         <v>16</v>
@@ -52155,7 +52155,7 @@
         <v>831</v>
       </c>
       <c r="H978" s="1" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
       <c r="I978" s="1"/>
       <c r="J978" s="1" t="s">
@@ -52194,7 +52194,7 @@
         <v>831</v>
       </c>
       <c r="H979" s="1" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
       <c r="I979" s="1"/>
       <c r="J979" s="1" t="s">
@@ -52233,7 +52233,7 @@
         <v>831</v>
       </c>
       <c r="H980" s="1" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
       <c r="I980" s="1"/>
       <c r="J980" s="1" t="s">
@@ -52272,7 +52272,7 @@
         <v>831</v>
       </c>
       <c r="H981" s="1" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="I981" s="1"/>
       <c r="J981" s="1" t="s">
@@ -52348,7 +52348,7 @@
         <v>789</v>
       </c>
       <c r="H983" s="1" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="I983" s="1"/>
       <c r="J983" s="1" t="s">
@@ -52387,7 +52387,7 @@
         <v>789</v>
       </c>
       <c r="H984" s="1" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
       <c r="I984" s="1"/>
       <c r="J984" s="1" t="s">
@@ -52426,7 +52426,7 @@
         <v>111</v>
       </c>
       <c r="H985" s="1" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
       <c r="I985" s="1"/>
       <c r="J985" s="1" t="s">
@@ -53450,7 +53450,7 @@
         <v>16</v>
       </c>
       <c r="J1007" s="1" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="K1007">
         <v>0</v>
@@ -53779,7 +53779,7 @@
         <v>16</v>
       </c>
       <c r="J1014" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="K1014" s="1">
         <v>3.3</v>
@@ -53920,7 +53920,7 @@
         <v>16</v>
       </c>
       <c r="J1017" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="K1017" s="1">
         <v>0</v>
@@ -53967,7 +53967,7 @@
         <v>16</v>
       </c>
       <c r="J1018" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
       <c r="K1018" s="1">
         <v>1.8</v>
@@ -54040,7 +54040,7 @@
         <v>844</v>
       </c>
       <c r="D1020" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="E1020" t="s">
         <v>16</v>
@@ -54052,7 +54052,7 @@
         <v>70</v>
       </c>
       <c r="H1020" s="1" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="I1020" t="s">
         <v>16</v>
@@ -54199,7 +54199,7 @@
         <v>757</v>
       </c>
       <c r="J1023" s="1" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="K1023" s="1">
         <v>4</v>
@@ -54528,7 +54528,7 @@
         <v>16</v>
       </c>
       <c r="J1030" s="1" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="K1030" s="1">
         <v>4</v>
@@ -54904,7 +54904,7 @@
         <v>16</v>
       </c>
       <c r="J1038" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="K1038" s="1">
         <v>5.3330000000000002</v>
@@ -54951,7 +54951,7 @@
         <v>16</v>
       </c>
       <c r="J1039" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="K1039">
         <v>5.3330000000000002</v>
@@ -55086,7 +55086,7 @@
         <v>278</v>
       </c>
       <c r="H1042" s="1" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
       <c r="I1042" s="1" t="s">
         <v>689</v>
@@ -55133,7 +55133,7 @@
         <v>278</v>
       </c>
       <c r="H1043" s="1" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
       <c r="I1043" s="1" t="s">
         <v>689</v>
@@ -55180,7 +55180,7 @@
         <v>278</v>
       </c>
       <c r="H1044" s="1" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
       <c r="I1044" s="1" t="s">
         <v>689</v>
@@ -55227,7 +55227,7 @@
         <v>278</v>
       </c>
       <c r="H1045" s="1" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="I1045" s="1" t="s">
         <v>689</v>
@@ -55274,7 +55274,7 @@
         <v>278</v>
       </c>
       <c r="H1046" s="1" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="I1046" s="1" t="s">
         <v>689</v>
@@ -55321,7 +55321,7 @@
         <v>278</v>
       </c>
       <c r="H1047" s="1" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="I1047" s="1" t="s">
         <v>689</v>
@@ -55368,7 +55368,7 @@
         <v>672</v>
       </c>
       <c r="H1048" s="1" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="I1048" t="s">
         <v>16</v>
@@ -55515,7 +55515,7 @@
         <v>16</v>
       </c>
       <c r="J1051" s="1" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="K1051" s="1">
         <v>0</v>
@@ -55603,7 +55603,7 @@
         <v>475</v>
       </c>
       <c r="H1053" s="1" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
       <c r="I1053" t="s">
         <v>16</v>
@@ -55791,7 +55791,7 @@
         <v>76</v>
       </c>
       <c r="H1057" s="1" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="I1057" t="s">
         <v>16</v>
@@ -55838,7 +55838,7 @@
         <v>76</v>
       </c>
       <c r="H1058" s="1" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="I1058" t="s">
         <v>16</v>
@@ -55885,7 +55885,7 @@
         <v>255</v>
       </c>
       <c r="H1059" s="1" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="I1059" t="s">
         <v>16</v>
@@ -55932,7 +55932,7 @@
         <v>87</v>
       </c>
       <c r="H1060" s="1" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="I1060" t="s">
         <v>16</v>
@@ -56020,7 +56020,7 @@
         <v>19</v>
       </c>
       <c r="H1062" s="1" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="I1062" t="s">
         <v>16</v>
@@ -56299,7 +56299,7 @@
         <v>20</v>
       </c>
       <c r="H1068" s="1" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="I1068" t="s">
         <v>16</v>
@@ -56346,13 +56346,13 @@
         <v>16</v>
       </c>
       <c r="H1069" s="1" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="I1069" t="s">
         <v>16</v>
       </c>
       <c r="J1069" s="1" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="K1069" s="1">
         <v>0</v>
@@ -56399,7 +56399,7 @@
         <v>16</v>
       </c>
       <c r="J1070" s="2" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="K1070" s="2">
         <v>1.17E-2</v>
@@ -56675,7 +56675,7 @@
         <v>255</v>
       </c>
       <c r="H1076" s="1" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="I1076" t="s">
         <v>16</v>
@@ -56769,7 +56769,7 @@
         <v>255</v>
       </c>
       <c r="H1078" s="1" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="I1078" t="s">
         <v>16</v>
@@ -56816,7 +56816,7 @@
         <v>255</v>
       </c>
       <c r="H1079" s="1" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="I1079" t="s">
         <v>16</v>
@@ -56863,7 +56863,7 @@
         <v>255</v>
       </c>
       <c r="H1080" s="1" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="I1080" t="s">
         <v>16</v>
@@ -56898,7 +56898,7 @@
         <v>885</v>
       </c>
       <c r="D1081" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
       <c r="E1081" t="s">
         <v>16</v>
@@ -56913,7 +56913,7 @@
         <v>886</v>
       </c>
       <c r="I1081" s="1" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
       <c r="J1081" s="1" t="s">
         <v>79</v>
@@ -57004,7 +57004,7 @@
         <v>100</v>
       </c>
       <c r="H1083" s="1" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
       <c r="I1083" t="s">
         <v>16</v>
@@ -57142,10 +57142,10 @@
         <v>19</v>
       </c>
       <c r="G1086" s="1" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
       <c r="H1086" s="1" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
       <c r="I1086" t="s">
         <v>16</v>
@@ -57333,7 +57333,7 @@
         <v>16</v>
       </c>
       <c r="H1090" s="1" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="I1090" t="s">
         <v>16</v>
@@ -57615,7 +57615,7 @@
         <v>76</v>
       </c>
       <c r="H1096" s="1" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
       <c r="I1096" s="1" t="s">
         <v>897</v>
@@ -57662,7 +57662,7 @@
         <v>416</v>
       </c>
       <c r="H1097" s="1" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
       <c r="I1097" t="s">
         <v>16</v>
@@ -57744,7 +57744,7 @@
         <v>901</v>
       </c>
       <c r="D1099" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="E1099" t="s">
         <v>18</v>
@@ -58085,7 +58085,7 @@
         <v>76</v>
       </c>
       <c r="H1106" s="1" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
       <c r="I1106" t="s">
         <v>16</v>
@@ -58179,13 +58179,13 @@
         <v>76</v>
       </c>
       <c r="H1108" s="1" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
       <c r="I1108" t="s">
         <v>16</v>
       </c>
       <c r="J1108" s="1" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
       <c r="K1108" s="1">
         <v>1.17E-2</v>
@@ -58226,7 +58226,7 @@
         <v>475</v>
       </c>
       <c r="H1109" s="1" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
       <c r="I1109" t="s">
         <v>16</v>
@@ -58508,7 +58508,7 @@
         <v>100</v>
       </c>
       <c r="H1115" s="1" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
       <c r="I1115" t="s">
         <v>16</v>
@@ -58555,7 +58555,7 @@
         <v>255</v>
       </c>
       <c r="H1116" s="1" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="I1116" t="s">
         <v>16</v>
@@ -58602,7 +58602,7 @@
         <v>255</v>
       </c>
       <c r="H1117" s="1" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="I1117" t="s">
         <v>16</v>
@@ -58825,7 +58825,7 @@
         <v>917</v>
       </c>
       <c r="D1122" t="s">
-        <v>1438</v>
+        <v>1437</v>
       </c>
       <c r="E1122" t="s">
         <v>16</v>

</xml_diff>